<commit_message>
Dossier Projet partie jeu d'essai et Réalisations C, correction US
</commit_message>
<xml_diff>
--- a/dossier_admin/admin/Dossier de Projet/divers/glossaire.xlsx
+++ b/dossier_admin/admin/Dossier de Projet/divers/glossaire.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dressingAngular\dossier_admin\admin\Dossier de Projet\divers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dressingAngular\dossier_admin\admin\Dossier de Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AEA29E-1E32-4443-9B7F-EB503BAF2056}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F08525D-5A46-4E3E-A1F3-43B13339592D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9BE8E046-0BB6-4C73-9833-F658CF36896D}"/>
+    <workbookView xWindow="4755" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{9BE8E046-0BB6-4C73-9833-F658CF36896D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -495,7 +495,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,7 +520,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -528,7 +528,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -560,7 +560,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -568,7 +568,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -576,7 +576,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -592,7 +592,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -600,7 +600,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Dossier projet mise en forme
</commit_message>
<xml_diff>
--- a/dossier_admin/admin/Dossier de Projet/divers/glossaire.xlsx
+++ b/dossier_admin/admin/Dossier de Projet/divers/glossaire.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dressingAngular\dossier_admin\admin\Dossier de Projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dressingAngular\dossier_admin\admin\Dossier de Projet\divers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F08525D-5A46-4E3E-A1F3-43B13339592D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9265B7DE-DB83-49C4-8E7E-D594BB8EF459}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4755" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{9BE8E046-0BB6-4C73-9833-F658CF36896D}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="26">
   <si>
     <t>Termes</t>
   </si>
@@ -114,13 +114,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,12 +149,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -157,12 +169,48 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -182,14 +230,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7BEE4A46-5961-4278-93E7-A3ACF3D411E0}" name="Tableau2" displayName="Tableau2" ref="A1:B13" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7BEE4A46-5961-4278-93E7-A3ACF3D411E0}" name="Tableau2" displayName="Tableau2" ref="A1:B13" totalsRowShown="0" headerRowDxfId="3" dataDxfId="0">
   <autoFilter ref="A1:B13" xr:uid="{ED6BB10D-BFC9-4B77-BB1B-4A8EA814378B}"/>
   <sortState ref="A2:B13">
     <sortCondition ref="A1:A13"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3B3615EB-ADE0-45D5-A9C5-D36E2331FA81}" name="Termes" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{A2250946-9479-42BB-8675-5C1346D6AAA9}" name="Définitions" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{3B3615EB-ADE0-45D5-A9C5-D36E2331FA81}" name="Termes" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{A2250946-9479-42BB-8675-5C1346D6AAA9}" name="Définitions" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -495,7 +543,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,105 +560,105 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
Dossier projet corrections, création fichiers maquette html/css
</commit_message>
<xml_diff>
--- a/dossier_admin/admin/Dossier de Projet/divers/glossaire.xlsx
+++ b/dossier_admin/admin/Dossier de Projet/divers/glossaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dressingAngular\dossier_admin\admin\Dossier de Projet\divers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9265B7DE-DB83-49C4-8E7E-D594BB8EF459}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3953DE-9E6A-4F31-8F88-42F1538DD4D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4755" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{9BE8E046-0BB6-4C73-9833-F658CF36896D}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Termes</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Marque</t>
   </si>
   <si>
-    <t>Catégorie à laquelle appartient un vêtement : pantalon, jupe, veste, tshirt, blouse… - un vêtement appartient à une seule catégorie. L'utilisateur peut ajouter des catégories.</t>
-  </si>
-  <si>
     <t>Couleur d'un vêtement - un vêtement peut avoir plusieurs couleurs. L'utilisateur peut ajouter des couleurs.</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>Marque d'un vêtement - un vêtement a une seule marque. L'utilisateur peut ajouter des marques.</t>
+  </si>
+  <si>
+    <t>Catégorie à laquelle appartient un vêtement : pantalon, jupe, veste, t-shirt, blouse… - un vêtement appartient à une seule catégorie. L'utilisateur peut ajouter des catégories.</t>
   </si>
 </sst>
 </file>
@@ -181,7 +181,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -196,7 +196,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -230,14 +230,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7BEE4A46-5961-4278-93E7-A3ACF3D411E0}" name="Tableau2" displayName="Tableau2" ref="A1:B13" totalsRowShown="0" headerRowDxfId="3" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7BEE4A46-5961-4278-93E7-A3ACF3D411E0}" name="Tableau2" displayName="Tableau2" ref="A1:B13" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B13" xr:uid="{ED6BB10D-BFC9-4B77-BB1B-4A8EA814378B}"/>
   <sortState ref="A2:B13">
     <sortCondition ref="A1:A13"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3B3615EB-ADE0-45D5-A9C5-D36E2331FA81}" name="Termes" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{A2250946-9479-42BB-8675-5C1346D6AAA9}" name="Définitions" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3B3615EB-ADE0-45D5-A9C5-D36E2331FA81}" name="Termes" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{A2250946-9479-42BB-8675-5C1346D6AAA9}" name="Définitions" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -543,7 +543,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +565,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
@@ -573,7 +573,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
@@ -581,23 +581,23 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
@@ -605,39 +605,39 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
@@ -645,15 +645,15 @@
         <v>2</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>